<commit_message>
Change MP3 module to DFPlayer Mini MP3 Player
</commit_message>
<xml_diff>
--- a/D1 mini pin-out.xlsx
+++ b/D1 mini pin-out.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Fouchet_F\Documents\FabLab\PontTournant\ESP8266\PontTournant\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Fouchet_F\Documents\FabLab\PontTournant\PontTournant\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D895ED97-4116-4AFD-9264-69B4EC8DE0C8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9DE2D99-B1B8-4B4D-9C68-1CD156ED79DF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="540" yWindow="2175" windowWidth="25425" windowHeight="13290" xr2:uid="{9681CD7C-A6E7-44E1-988E-193C12B07DDC}"/>
+    <workbookView xWindow="4110" yWindow="2310" windowWidth="22935" windowHeight="13290" xr2:uid="{9681CD7C-A6E7-44E1-988E-193C12B07DDC}"/>
   </bookViews>
   <sheets>
     <sheet name="Pin" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="85">
   <si>
     <t>Pin</t>
   </si>
@@ -258,9 +258,6 @@
     <t>USB</t>
   </si>
   <si>
-    <t>MP3 module</t>
-  </si>
-  <si>
     <t>LED</t>
   </si>
   <si>
@@ -277,6 +274,12 @@
   </si>
   <si>
     <t>Stepper direction</t>
+  </si>
+  <si>
+    <t>MP3 TX</t>
+  </si>
+  <si>
+    <t>MP3 RX</t>
   </si>
 </sst>
 </file>
@@ -690,7 +693,7 @@
   <dimension ref="A1:H23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N3" sqref="N3"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -806,7 +809,7 @@
       </c>
       <c r="F5" s="5"/>
       <c r="H5" s="7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -823,8 +826,8 @@
       <c r="F6" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="H6" s="7" t="s">
-        <v>82</v>
+      <c r="H6" s="12" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -843,8 +846,8 @@
         <v>71</v>
       </c>
       <c r="G7" s="6"/>
-      <c r="H7" s="7" t="s">
-        <v>83</v>
+      <c r="H7" s="12" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -868,7 +871,7 @@
         <v>74</v>
       </c>
       <c r="H8" s="7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -889,9 +892,7 @@
       </c>
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
-      <c r="H9" s="7" t="s">
-        <v>77</v>
-      </c>
+      <c r="H9" s="7"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
@@ -907,7 +908,7 @@
       </c>
       <c r="G10" s="3"/>
       <c r="H10" s="7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -925,7 +926,7 @@
       <c r="F11" s="5"/>
       <c r="G11" s="3"/>
       <c r="H11" s="7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -943,8 +944,8 @@
       <c r="G12" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="H12" s="12" t="s">
-        <v>32</v>
+      <c r="H12" s="7" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -967,8 +968,8 @@
         <v>72</v>
       </c>
       <c r="G13" s="13"/>
-      <c r="H13" s="12" t="s">
-        <v>32</v>
+      <c r="H13" s="7" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>